<commit_message>
re-factor flujos y sus keywords
</commit_message>
<xml_diff>
--- a/External Resources/UI/Cupo/CasosPruebaValidarCupo.xlsx
+++ b/External Resources/UI/Cupo/CasosPruebaValidarCupo.xlsx
@@ -567,7 +567,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F17" sqref="F17"/>
+      <selection pane="bottomLeft" activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2423,7 +2423,9 @@
       <c r="J30" s="4"/>
       <c r="K30" s="4"/>
       <c r="L30" s="4"/>
-      <c r="M30" s="4"/>
+      <c r="M30" s="4" t="b">
+        <v>0</v>
+      </c>
       <c r="N30" s="4"/>
       <c r="O30" s="5"/>
       <c r="P30" s="5"/>
@@ -2447,6 +2449,9 @@
         <v>888811111129</v>
       </c>
       <c r="D31" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="M31" s="4" t="b">
         <v>0</v>
       </c>
       <c r="V31" s="4">
@@ -4326,7 +4331,9 @@
       <c r="J30" s="4"/>
       <c r="K30" s="4"/>
       <c r="L30" s="4"/>
-      <c r="M30" s="4"/>
+      <c r="M30" s="4" t="b">
+        <v>0</v>
+      </c>
       <c r="N30" s="4"/>
       <c r="O30" s="5"/>
       <c r="P30" s="5"/>
@@ -4352,6 +4359,9 @@
       <c r="D31" s="3" t="b">
         <v>0</v>
       </c>
+      <c r="M31" s="4" t="b">
+        <v>0</v>
+      </c>
       <c r="V31" s="4">
         <v>1</v>
       </c>

</xml_diff>

<commit_message>
Test de circuitos levantando info de excel
</commit_message>
<xml_diff>
--- a/External Resources/UI/Cupo/CasosPruebaValidarCupo.xlsx
+++ b/External Resources/UI/Cupo/CasosPruebaValidarCupo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fabio.olivieri\RobotTesting\YARD\External Resources\UI\Cupo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{830ED6CA-9DA9-4E81-A475-6F4D6D5A28BE}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAEEC2E6-82A4-4145-B61E-575814445A04}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -609,7 +609,7 @@
   <dimension ref="A1:X31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
@@ -2517,8 +2517,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:X31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView topLeftCell="N1" workbookViewId="0">
+      <selection activeCell="N1" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>